<commit_message>
updated clinic template, deleted test template
</commit_message>
<xml_diff>
--- a/Clinic_Template.xlsx
+++ b/Clinic_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminrutherford/Documents/School/Main Campus/ECE435/ece435/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delaneyheileman/Documents/school/spring 2021/435/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BB5A4CE-5809-554D-AAF9-7D71A6CDB2AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14BD97D-F017-0142-ABF1-28C73683010F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,44 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Clinic Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Number of Pediatric Doctors Needed </t>
+  </si>
+  <si>
+    <t>Min Number of Adult Doctors Needed</t>
+  </si>
+  <si>
+    <t>Ideal # of Providers</t>
+  </si>
+  <si>
+    <t>Max # of Providers</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,8 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +413,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0370FC8E-AF66-8E44-85E1-006964A21BFE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
deleted weird xml files
</commit_message>
<xml_diff>
--- a/Clinic_Template.xlsx
+++ b/Clinic_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delaneyheileman/Documents/school/spring 2021/435/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276B088-BB0B-694F-A75A-36B918D9A3F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E93D928-7B8D-3C46-9F57-2E401A28A8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-22280" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
   </bookViews>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated clinic sheet to match class
</commit_message>
<xml_diff>
--- a/Clinic_Template.xlsx
+++ b/Clinic_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delaneyheileman/Documents/school/spring 2021/435/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E93D928-7B8D-3C46-9F57-2E401A28A8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B462B-C3C9-BE44-8387-D5F5001226FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-22280" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Clinic Name</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Min Number of Adult Doctors Needed</t>
   </si>
   <si>
-    <t>Ideal # of Providers</t>
-  </si>
-  <si>
     <t>Max # of Providers</t>
   </si>
   <si>
@@ -58,13 +55,19 @@
   </si>
   <si>
     <t>Pueblo Pintado Health Center</t>
+  </si>
+  <si>
+    <t>Ideal ped</t>
+  </si>
+  <si>
+    <t>ideal adult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,6 +83,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,13 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -425,69 +436,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0370FC8E-AF66-8E44-85E1-006964A21BFE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="B4">
         <v>1</v>
       </c>
@@ -495,9 +515,12 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated clinic ideal numbers
</commit_message>
<xml_diff>
--- a/Clinic_Template.xlsx
+++ b/Clinic_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delaneyheileman/Documents/school/spring 2021/435/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B462B-C3C9-BE44-8387-D5F5001226FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39BD508-EB83-124C-8688-F31AC48C6BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -495,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>3</v>

</xml_diff>

<commit_message>
final version for pres
</commit_message>
<xml_diff>
--- a/Clinic_Template.xlsx
+++ b/Clinic_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/delaneyheileman/Documents/school/spring 2021/435/ece435/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminrutherford/PycharmProjects/ece435/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39BD508-EB83-124C-8688-F31AC48C6BAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7738F27C-917D-0C44-AB33-BAB13FBC3E16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
+    <workbookView xWindow="15460" yWindow="1760" windowWidth="14280" windowHeight="18000" xr2:uid="{87625C3B-A9C9-8A4B-BCC7-5753D8E10EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,19 +48,19 @@
     <t>Max # of Providers</t>
   </si>
   <si>
-    <t>Crownpoint Healthcare Facility</t>
-  </si>
-  <si>
-    <t>Thoreau Health Station (THS)</t>
-  </si>
-  <si>
-    <t>Pueblo Pintado Health Center</t>
-  </si>
-  <si>
     <t>Ideal ped</t>
   </si>
   <si>
     <t>ideal adult</t>
+  </si>
+  <si>
+    <t>CHCF</t>
+  </si>
+  <si>
+    <t>THS</t>
+  </si>
+  <si>
+    <t>PPH</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,18 +455,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -484,9 +484,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -495,18 +495,18 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -515,10 +515,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>3</v>

</xml_diff>